<commit_message>
now faculty can assign different sets to the students
</commit_message>
<xml_diff>
--- a/onlineproctore/public/DashboardFaculty/downloads/upload_questions.xlsx
+++ b/onlineproctore/public/DashboardFaculty/downloads/upload_questions.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iasdi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865B03E0-E7DE-4636-9194-4052B7D28E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCCF676-4797-45D2-A69D-1F1AB1E01D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB20542C-6F78-464B-875C-C1D6BE86CEA4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>S.No.</t>
   </si>
@@ -100,6 +100,51 @@
   </si>
   <si>
     <t>explain in points</t>
+  </si>
+  <si>
+    <t>ImageLink1</t>
+  </si>
+  <si>
+    <t>ImageLink2</t>
+  </si>
+  <si>
+    <t>ImageLink3</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1W9KY0Pd33L1XavWug8haqdOE17EMYT73/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1MKZkLsTZjarMPMyW6Zg4DaVZG4GR9fZ_/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1a5j94WsGrc1_5vCuDZ7f66KhGV6ax4il/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1WM1qMZnu-QO1gvWmZKQeal8pxDZU-mn8/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>What is full form of AGA?</t>
+  </si>
+  <si>
+    <t>What is image enhancement?</t>
+  </si>
+  <si>
+    <t>Full form of AGA is Advanced graphics animation?</t>
+  </si>
+  <si>
+    <t>Which of the following are Image Enhancement Techniques?</t>
+  </si>
+  <si>
+    <t>Retinex</t>
+  </si>
+  <si>
+    <t>HE</t>
+  </si>
+  <si>
+    <t>LOG Transformation</t>
   </si>
 </sst>
 </file>
@@ -115,15 +160,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,12 +182,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,153 +519,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B8808E-903D-4E82-BFBF-068965C850E6}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
     <col min="3" max="3" width="54.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3">
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K4">
+      <c r="O4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K5">
+      <c r="O5" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="1">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
now faculty can decide which question can be given as typed or handwritten corresponding to which file upload option will appear at the end
</commit_message>
<xml_diff>
--- a/onlineproctore/public/DashboardFaculty/downloads/upload_questions.xlsx
+++ b/onlineproctore/public/DashboardFaculty/downloads/upload_questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iasdi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCCF676-4797-45D2-A69D-1F1AB1E01D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FF81FA-FF91-41C2-8E82-7F62BDD418FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB20542C-6F78-464B-875C-C1D6BE86CEA4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>S.No.</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>LOG Transformation</t>
+  </si>
+  <si>
+    <t>PdfUpload</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B8808E-903D-4E82-BFBF-068965C850E6}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,20 +533,20 @@
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
     <col min="3" max="3" width="54.6640625" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,37 +563,40 @@
         <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -607,19 +613,22 @@
         <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -636,19 +645,22 @@
         <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -662,34 +674,37 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="2">
-        <v>2</v>
-      </c>
-      <c r="J4" s="2" t="b">
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="2" t="b">
+      <c r="L4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>1</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -703,37 +718,40 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -750,19 +768,22 @@
         <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -779,19 +800,22 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -805,34 +829,37 @@
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="1">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1" t="b">
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="K8" s="1" t="b">
+      <c r="L8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>1</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -846,33 +873,36 @@
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>3</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P9" s="1">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>